<commit_message>
add forecast and updated keras file
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttbon\Desktop\stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F71CBE-A6DA-462F-AFBC-81C3A1C71A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977D2B35-CAEE-4A79-8D45-C4BE9942F688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="255" windowWidth="12405" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="1785" windowWidth="21600" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tickers" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13010" uniqueCount="8597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13054" uniqueCount="8597">
   <si>
     <t>tickers</t>
   </si>
@@ -56401,8 +56401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA55E37D-5D70-4D70-8000-B4CA16A6A6A0}">
   <dimension ref="A1:H1345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="H305" sqref="H305:H343"/>
+    <sheetView tabSelected="1" topLeftCell="A352" workbookViewId="0">
+      <selection activeCell="H345" sqref="H345:H388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64680,6 +64680,13 @@
       <c r="F346" t="s">
         <v>7576</v>
       </c>
+      <c r="G346" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H346" t="str">
+        <f t="shared" ref="H346:H363" si="16">_xlfn.CONCAT(F346,G346)</f>
+        <v>fad_history.csv</v>
+      </c>
     </row>
     <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
@@ -64697,6 +64704,13 @@
       <c r="F347" t="s">
         <v>7577</v>
       </c>
+      <c r="G347" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H347" t="str">
+        <f t="shared" si="16"/>
+        <v>fam_history.csv</v>
+      </c>
     </row>
     <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
@@ -64714,6 +64728,13 @@
       <c r="F348" t="s">
         <v>7578</v>
       </c>
+      <c r="G348" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H348" t="str">
+        <f t="shared" si="16"/>
+        <v>fan_history.csv</v>
+      </c>
     </row>
     <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
@@ -64731,6 +64752,13 @@
       <c r="F349" t="s">
         <v>7579</v>
       </c>
+      <c r="G349" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H349" t="str">
+        <f t="shared" si="16"/>
+        <v>fas_history.csv</v>
+      </c>
     </row>
     <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
@@ -64748,6 +64776,13 @@
       <c r="F350" t="s">
         <v>7580</v>
       </c>
+      <c r="G350" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H350" t="str">
+        <f t="shared" si="16"/>
+        <v>faus_history.csv</v>
+      </c>
     </row>
     <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
@@ -64765,6 +64800,13 @@
       <c r="F351" t="s">
         <v>7581</v>
       </c>
+      <c r="G351" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H351" t="str">
+        <f t="shared" si="16"/>
+        <v>faz_history.csv</v>
+      </c>
     </row>
     <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
@@ -64782,8 +64824,15 @@
       <c r="F352" t="s">
         <v>7582</v>
       </c>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G352" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H352" t="str">
+        <f t="shared" si="16"/>
+        <v>fbgx_history.csv</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>6237</v>
       </c>
@@ -64799,8 +64848,15 @@
       <c r="F353" t="s">
         <v>7583</v>
       </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G353" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H353" t="str">
+        <f t="shared" si="16"/>
+        <v>fbnd_history.csv</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>6238</v>
       </c>
@@ -64816,8 +64872,15 @@
       <c r="F354" t="s">
         <v>7584</v>
       </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G354" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H354" t="str">
+        <f t="shared" si="16"/>
+        <v>fbt_history.csv</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>6239</v>
       </c>
@@ -64833,8 +64896,15 @@
       <c r="F355" t="s">
         <v>7585</v>
       </c>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G355" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H355" t="str">
+        <f t="shared" si="16"/>
+        <v>fbz_history.csv</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>6240</v>
       </c>
@@ -64850,8 +64920,15 @@
       <c r="F356" t="s">
         <v>7586</v>
       </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G356" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H356" t="str">
+        <f t="shared" si="16"/>
+        <v>fca_history.csv</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>6241</v>
       </c>
@@ -64867,8 +64944,15 @@
       <c r="F357" t="s">
         <v>7587</v>
       </c>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G357" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H357" t="str">
+        <f t="shared" si="16"/>
+        <v>fcan_history.csv</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>6242</v>
       </c>
@@ -64884,8 +64968,15 @@
       <c r="F358" t="s">
         <v>7588</v>
       </c>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G358" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H358" t="str">
+        <f t="shared" si="16"/>
+        <v>fcg_history.csv</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>6243</v>
       </c>
@@ -64901,8 +64992,15 @@
       <c r="F359" t="s">
         <v>7589</v>
       </c>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G359" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H359" t="str">
+        <f t="shared" si="16"/>
+        <v>fcom_history.csv</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>6244</v>
       </c>
@@ -64918,8 +65016,15 @@
       <c r="F360" t="s">
         <v>7590</v>
       </c>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G360" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H360" t="str">
+        <f t="shared" si="16"/>
+        <v>fcor_history.csv</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>6245</v>
       </c>
@@ -64935,8 +65040,15 @@
       <c r="F361" t="s">
         <v>7591</v>
       </c>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G361" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H361" t="str">
+        <f t="shared" si="16"/>
+        <v>fct_history.csv</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>6246</v>
       </c>
@@ -64952,8 +65064,15 @@
       <c r="F362" t="s">
         <v>7592</v>
       </c>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G362" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H362" t="str">
+        <f t="shared" si="16"/>
+        <v>fdd_history.csv</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>6247</v>
       </c>
@@ -64969,8 +65088,15 @@
       <c r="F363" t="s">
         <v>7593</v>
       </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G363" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H363" t="str">
+        <f t="shared" si="16"/>
+        <v>fdis_history.csv</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>6248</v>
       </c>
@@ -64986,8 +65112,15 @@
       <c r="F364" t="s">
         <v>7594</v>
       </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G364" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H364" t="str">
+        <f t="shared" ref="H364:H366" si="17">_xlfn.CONCAT(F364,G364)</f>
+        <v>fdiv_history.csv</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>6249</v>
       </c>
@@ -65003,8 +65136,15 @@
       <c r="F365" t="s">
         <v>7595</v>
       </c>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G365" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H365" t="str">
+        <f t="shared" si="17"/>
+        <v>fdl_history.csv</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>6250</v>
       </c>
@@ -65020,8 +65160,15 @@
       <c r="F366" t="s">
         <v>7596</v>
       </c>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G366" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H366" t="str">
+        <f t="shared" si="17"/>
+        <v>fdm_history.csv</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>6251</v>
       </c>
@@ -65037,8 +65184,15 @@
       <c r="F367" t="s">
         <v>7597</v>
       </c>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G367" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H367" t="str">
+        <f t="shared" ref="H367:H383" si="18">_xlfn.CONCAT(F367,G367)</f>
+        <v>fdn_history.csv</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>6252</v>
       </c>
@@ -65054,8 +65208,15 @@
       <c r="F368" t="s">
         <v>7598</v>
       </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G368" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H368" t="str">
+        <f t="shared" si="18"/>
+        <v>fdt_history.csv</v>
+      </c>
+    </row>
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>6253</v>
       </c>
@@ -65071,8 +65232,15 @@
       <c r="F369" t="s">
         <v>7599</v>
       </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G369" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H369" t="str">
+        <f t="shared" si="18"/>
+        <v>fdts_history.csv</v>
+      </c>
+    </row>
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>6254</v>
       </c>
@@ -65088,8 +65256,15 @@
       <c r="F370" t="s">
         <v>7600</v>
       </c>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G370" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H370" t="str">
+        <f t="shared" si="18"/>
+        <v>feeu_history.csv</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>6255</v>
       </c>
@@ -65105,8 +65280,15 @@
       <c r="F371" t="s">
         <v>7601</v>
       </c>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G371" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H371" t="str">
+        <f t="shared" si="18"/>
+        <v>fei_history.csv</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>6256</v>
       </c>
@@ -65122,8 +65304,15 @@
       <c r="F372" t="s">
         <v>7602</v>
       </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G372" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H372" t="str">
+        <f t="shared" si="18"/>
+        <v>fem_history.csv</v>
+      </c>
+    </row>
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>6257</v>
       </c>
@@ -65139,8 +65328,15 @@
       <c r="F373" t="s">
         <v>7603</v>
       </c>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G373" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H373" t="str">
+        <f t="shared" si="18"/>
+        <v>femb_history.csv</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>6258</v>
       </c>
@@ -65156,8 +65352,15 @@
       <c r="F374" t="s">
         <v>7604</v>
       </c>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G374" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H374" t="str">
+        <f t="shared" si="18"/>
+        <v>fems_history.csv</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>6259</v>
       </c>
@@ -65173,8 +65376,15 @@
       <c r="F375" t="s">
         <v>7605</v>
       </c>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G375" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H375" t="str">
+        <f t="shared" si="18"/>
+        <v>feny_history.csv</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>6260</v>
       </c>
@@ -65190,8 +65400,15 @@
       <c r="F376" t="s">
         <v>7606</v>
       </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G376" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H376" t="str">
+        <f t="shared" si="18"/>
+        <v>feo_history.csv</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>6261</v>
       </c>
@@ -65207,8 +65424,15 @@
       <c r="F377" t="s">
         <v>7607</v>
       </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G377" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H377" t="str">
+        <f t="shared" si="18"/>
+        <v>fep_history.csv</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>6262</v>
       </c>
@@ -65224,8 +65448,15 @@
       <c r="F378" t="s">
         <v>7608</v>
       </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G378" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H378" t="str">
+        <f t="shared" si="18"/>
+        <v>feu_history.csv</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>6263</v>
       </c>
@@ -65241,8 +65472,15 @@
       <c r="F379" t="s">
         <v>7609</v>
       </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G379" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H379" t="str">
+        <f t="shared" si="18"/>
+        <v>feuz_history.csv</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>6264</v>
       </c>
@@ -65258,8 +65496,15 @@
       <c r="F380" t="s">
         <v>7610</v>
       </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G380" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H380" t="str">
+        <f t="shared" si="18"/>
+        <v>fex_history.csv</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>6265</v>
       </c>
@@ -65275,8 +65520,15 @@
       <c r="F381" t="s">
         <v>7611</v>
       </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G381" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H381" t="str">
+        <f t="shared" si="18"/>
+        <v>fez_history.csv</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>6266</v>
       </c>
@@ -65292,8 +65544,15 @@
       <c r="F382" t="s">
         <v>7612</v>
       </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G382" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H382" t="str">
+        <f t="shared" si="18"/>
+        <v>ffa_history.csv</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>6267</v>
       </c>
@@ -65309,8 +65568,15 @@
       <c r="F383" t="s">
         <v>7613</v>
       </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G383" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H383" t="str">
+        <f t="shared" si="18"/>
+        <v>ffr_history.csv</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>6268</v>
       </c>
@@ -65326,8 +65592,15 @@
       <c r="F384" t="s">
         <v>7614</v>
       </c>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G384" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H384" t="str">
+        <f t="shared" ref="H384:H390" si="19">_xlfn.CONCAT(F384,G384)</f>
+        <v>fgb_history.csv</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>6269</v>
       </c>
@@ -65343,8 +65616,15 @@
       <c r="F385" t="s">
         <v>7615</v>
       </c>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G385" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H385" t="str">
+        <f t="shared" si="19"/>
+        <v>fgd_history.csv</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>6270</v>
       </c>
@@ -65360,8 +65640,15 @@
       <c r="F386" t="s">
         <v>7616</v>
       </c>
-    </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G386" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H386" t="str">
+        <f t="shared" si="19"/>
+        <v>fgm_history.csv</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>6271</v>
       </c>
@@ -65377,8 +65664,15 @@
       <c r="F387" t="s">
         <v>7617</v>
       </c>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G387" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H387" t="str">
+        <f t="shared" si="19"/>
+        <v>fhk_history.csv</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>6272</v>
       </c>
@@ -65391,11 +65685,18 @@
       <c r="D388" t="s">
         <v>7232</v>
       </c>
-      <c r="F388" t="s">
+      <c r="F388" s="2" t="s">
         <v>7618</v>
       </c>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G388" s="2" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H388" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>fhlc_history.csv</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>6273</v>
       </c>
@@ -65412,7 +65713,7 @@
         <v>7619</v>
       </c>
     </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>6274</v>
       </c>
@@ -65428,8 +65729,15 @@
       <c r="F390" t="s">
         <v>7620</v>
       </c>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G390" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H390" t="str">
+        <f t="shared" si="19"/>
+        <v>fidu_history.csv</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>6275</v>
       </c>
@@ -65446,7 +65754,7 @@
         <v>7621</v>
       </c>
     </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>6276</v>
       </c>
@@ -65463,7 +65771,7 @@
         <v>7622</v>
       </c>
     </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>6277</v>
       </c>
@@ -65480,7 +65788,7 @@
         <v>7623</v>
       </c>
     </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>6278</v>
       </c>
@@ -65497,7 +65805,7 @@
         <v>7624</v>
       </c>
     </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>6279</v>
       </c>
@@ -65514,7 +65822,7 @@
         <v>7625</v>
       </c>
     </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>6280</v>
       </c>
@@ -65531,7 +65839,7 @@
         <v>7626</v>
       </c>
     </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>6281</v>
       </c>
@@ -65548,7 +65856,7 @@
         <v>7627</v>
       </c>
     </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>6282</v>
       </c>
@@ -65565,7 +65873,7 @@
         <v>7628</v>
       </c>
     </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>6283</v>
       </c>
@@ -65582,7 +65890,7 @@
         <v>7629</v>
       </c>
     </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>6284</v>
       </c>

</xml_diff>

<commit_message>
moved prediction graph to front
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttbon\Desktop\stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB13935A-FDB2-43E5-A643-73A14E9A92EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C85242E-DC9B-44C7-B668-6A544B4B7C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="1320" windowWidth="21600" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4470" yWindow="1620" windowWidth="16080" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tickers" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13104" uniqueCount="8597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13205" uniqueCount="8598">
   <si>
     <t>tickers</t>
   </si>
@@ -25826,6 +25826,9 @@
   </si>
   <si>
     <t>AER_history.csv</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -56401,8 +56404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA55E37D-5D70-4D70-8000-B4CA16A6A6A0}">
   <dimension ref="A1:H1345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A429" workbookViewId="0">
-      <selection activeCell="H439" sqref="H390:H439"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="E491" sqref="E491"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66953,6 +66956,13 @@
       <c r="F441" t="s">
         <v>7671</v>
       </c>
+      <c r="G441" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H441" t="str">
+        <f t="shared" ref="H441:H453" si="22">_xlfn.CONCAT(F441,G441)</f>
+        <v>fsta_history.csv</v>
+      </c>
     </row>
     <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
@@ -66970,6 +66980,13 @@
       <c r="F442" t="s">
         <v>7672</v>
       </c>
+      <c r="G442" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H442" t="str">
+        <f t="shared" si="22"/>
+        <v>fsz_history.csv</v>
+      </c>
     </row>
     <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
@@ -66987,6 +67004,13 @@
       <c r="F443" t="s">
         <v>7673</v>
       </c>
+      <c r="G443" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H443" t="str">
+        <f t="shared" si="22"/>
+        <v>fta_history.csv</v>
+      </c>
     </row>
     <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
@@ -67004,6 +67028,13 @@
       <c r="F444" t="s">
         <v>7674</v>
       </c>
+      <c r="G444" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H444" t="str">
+        <f t="shared" si="22"/>
+        <v>ftc_history.csv</v>
+      </c>
     </row>
     <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
@@ -67021,6 +67052,13 @@
       <c r="F445" t="s">
         <v>7675</v>
       </c>
+      <c r="G445" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H445" t="str">
+        <f t="shared" si="22"/>
+        <v>ftcs_history.csv</v>
+      </c>
     </row>
     <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
@@ -67038,6 +67076,13 @@
       <c r="F446" t="s">
         <v>7676</v>
       </c>
+      <c r="G446" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H446" t="str">
+        <f t="shared" si="22"/>
+        <v>ftec_history.csv</v>
+      </c>
     </row>
     <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
@@ -67055,6 +67100,13 @@
       <c r="F447" t="s">
         <v>7677</v>
       </c>
+      <c r="G447" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H447" t="str">
+        <f t="shared" si="22"/>
+        <v>ftgc_history.csv</v>
+      </c>
     </row>
     <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
@@ -67072,8 +67124,15 @@
       <c r="F448" t="s">
         <v>7678</v>
       </c>
-    </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G448" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H448" t="str">
+        <f t="shared" si="22"/>
+        <v>fthi_history.csv</v>
+      </c>
+    </row>
+    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>6333</v>
       </c>
@@ -67089,8 +67148,15 @@
       <c r="F449" t="s">
         <v>7679</v>
       </c>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G449" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H449" t="str">
+        <f t="shared" si="22"/>
+        <v>ftlb_history.csv</v>
+      </c>
+    </row>
+    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>6334</v>
       </c>
@@ -67106,8 +67172,15 @@
       <c r="F450" t="s">
         <v>7680</v>
       </c>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G450" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H450" t="str">
+        <f t="shared" si="22"/>
+        <v>ftls_history.csv</v>
+      </c>
+    </row>
+    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>6335</v>
       </c>
@@ -67123,8 +67196,15 @@
       <c r="F451" t="s">
         <v>7681</v>
       </c>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G451" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H451" t="str">
+        <f t="shared" si="22"/>
+        <v>ftsd_history.csv</v>
+      </c>
+    </row>
+    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>6336</v>
       </c>
@@ -67140,8 +67220,15 @@
       <c r="F452" t="s">
         <v>7682</v>
       </c>
-    </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G452" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H452" t="str">
+        <f t="shared" si="22"/>
+        <v>ftsl_history.csv</v>
+      </c>
+    </row>
+    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>6337</v>
       </c>
@@ -67157,8 +67244,15 @@
       <c r="F453" t="s">
         <v>7683</v>
       </c>
-    </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G453" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H453" t="str">
+        <f t="shared" si="22"/>
+        <v>ftsm_history.csv</v>
+      </c>
+    </row>
+    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>6338</v>
       </c>
@@ -67175,7 +67269,7 @@
         <v>7684</v>
       </c>
     </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>6339</v>
       </c>
@@ -67191,8 +67285,15 @@
       <c r="F455" t="s">
         <v>7685</v>
       </c>
-    </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G455" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H455" t="str">
+        <f t="shared" ref="H454:H455" si="23">_xlfn.CONCAT(F455,G455)</f>
+        <v>fud_history.csv</v>
+      </c>
+    </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>6340</v>
       </c>
@@ -67208,8 +67309,15 @@
       <c r="F456" t="s">
         <v>7686</v>
       </c>
-    </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G456" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H456" t="str">
+        <f t="shared" ref="H456:H463" si="24">_xlfn.CONCAT(F456,G456)</f>
+        <v>fue_history.csv</v>
+      </c>
+    </row>
+    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>6341</v>
       </c>
@@ -67225,8 +67333,15 @@
       <c r="F457" t="s">
         <v>7687</v>
       </c>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G457" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H457" t="str">
+        <f t="shared" si="24"/>
+        <v>futy_history.csv</v>
+      </c>
+    </row>
+    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>6342</v>
       </c>
@@ -67242,8 +67357,15 @@
       <c r="F458" t="s">
         <v>7688</v>
       </c>
-    </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G458" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H458" t="str">
+        <f t="shared" si="24"/>
+        <v>fv_history.csv</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>6343</v>
       </c>
@@ -67259,8 +67381,15 @@
       <c r="F459" t="s">
         <v>7689</v>
       </c>
-    </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G459" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H459" t="str">
+        <f t="shared" si="24"/>
+        <v>fvd_history.csv</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>6344</v>
       </c>
@@ -67276,8 +67405,15 @@
       <c r="F460" t="s">
         <v>7690</v>
       </c>
-    </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G460" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H460" t="str">
+        <f t="shared" si="24"/>
+        <v>fvl_history.csv</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>6345</v>
       </c>
@@ -67293,8 +67429,15 @@
       <c r="F461" t="s">
         <v>7691</v>
       </c>
-    </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G461" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H461" t="str">
+        <f t="shared" si="24"/>
+        <v>fwdb_history.csv</v>
+      </c>
+    </row>
+    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>6346</v>
       </c>
@@ -67310,8 +67453,15 @@
       <c r="F462" t="s">
         <v>7692</v>
       </c>
-    </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G462" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H462" t="str">
+        <f t="shared" si="24"/>
+        <v>fwdd_history.csv</v>
+      </c>
+    </row>
+    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>6347</v>
       </c>
@@ -67327,8 +67477,15 @@
       <c r="F463" t="s">
         <v>7693</v>
       </c>
-    </row>
-    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G463" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H463" t="str">
+        <f t="shared" si="24"/>
+        <v>fwdi_history.csv</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>6348</v>
       </c>
@@ -67344,8 +67501,15 @@
       <c r="F464" t="s">
         <v>7694</v>
       </c>
-    </row>
-    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G464" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H464" t="str">
+        <f t="shared" ref="H464:H471" si="25">_xlfn.CONCAT(F464,G464)</f>
+        <v>fxa_history.csv</v>
+      </c>
+    </row>
+    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>6349</v>
       </c>
@@ -67361,8 +67525,15 @@
       <c r="F465" t="s">
         <v>7695</v>
       </c>
-    </row>
-    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G465" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H465" t="str">
+        <f t="shared" si="25"/>
+        <v>fxb_history.csv</v>
+      </c>
+    </row>
+    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>6350</v>
       </c>
@@ -67378,8 +67549,15 @@
       <c r="F466" t="s">
         <v>7696</v>
       </c>
-    </row>
-    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G466" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H466" t="str">
+        <f t="shared" si="25"/>
+        <v>fxc_history.csv</v>
+      </c>
+    </row>
+    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>6351</v>
       </c>
@@ -67395,8 +67573,15 @@
       <c r="F467" t="s">
         <v>7697</v>
       </c>
-    </row>
-    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G467" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H467" t="str">
+        <f t="shared" si="25"/>
+        <v>fxch_history.csv</v>
+      </c>
+    </row>
+    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>6352</v>
       </c>
@@ -67412,8 +67597,15 @@
       <c r="F468" t="s">
         <v>7698</v>
       </c>
-    </row>
-    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G468" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H468" t="str">
+        <f t="shared" si="25"/>
+        <v>fxd_history.csv</v>
+      </c>
+    </row>
+    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>6353</v>
       </c>
@@ -67429,8 +67621,15 @@
       <c r="F469" t="s">
         <v>7699</v>
       </c>
-    </row>
-    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G469" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H469" t="str">
+        <f t="shared" si="25"/>
+        <v>fxe_history.csv</v>
+      </c>
+    </row>
+    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>6354</v>
       </c>
@@ -67446,8 +67645,15 @@
       <c r="F470" t="s">
         <v>7700</v>
       </c>
-    </row>
-    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G470" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H470" t="str">
+        <f t="shared" si="25"/>
+        <v>fxeu_history.csv</v>
+      </c>
+    </row>
+    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>6355</v>
       </c>
@@ -67463,8 +67669,15 @@
       <c r="F471" t="s">
         <v>7701</v>
       </c>
-    </row>
-    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G471" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H471" t="str">
+        <f t="shared" si="25"/>
+        <v>fxf_history.csv</v>
+      </c>
+    </row>
+    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>6356</v>
       </c>
@@ -67480,8 +67693,15 @@
       <c r="F472" t="s">
         <v>7702</v>
       </c>
-    </row>
-    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G472" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H472" t="str">
+        <f t="shared" ref="H472:H490" si="26">_xlfn.CONCAT(F472,G472)</f>
+        <v>fxg_history.csv</v>
+      </c>
+    </row>
+    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>6357</v>
       </c>
@@ -67497,8 +67717,15 @@
       <c r="F473" t="s">
         <v>7703</v>
       </c>
-    </row>
-    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G473" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H473" t="str">
+        <f t="shared" si="26"/>
+        <v>fxh_history.csv</v>
+      </c>
+    </row>
+    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>6358</v>
       </c>
@@ -67514,8 +67741,15 @@
       <c r="F474" t="s">
         <v>7704</v>
       </c>
-    </row>
-    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G474" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H474" t="str">
+        <f t="shared" si="26"/>
+        <v>fxi_history.csv</v>
+      </c>
+    </row>
+    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>6359</v>
       </c>
@@ -67531,8 +67765,15 @@
       <c r="F475" t="s">
         <v>7705</v>
       </c>
-    </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G475" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H475" t="str">
+        <f t="shared" si="26"/>
+        <v>fxl_history.csv</v>
+      </c>
+    </row>
+    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>6360</v>
       </c>
@@ -67548,8 +67789,15 @@
       <c r="F476" t="s">
         <v>7706</v>
       </c>
-    </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G476" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H476" t="str">
+        <f t="shared" si="26"/>
+        <v>fxn_history.csv</v>
+      </c>
+    </row>
+    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>6361</v>
       </c>
@@ -67565,8 +67813,15 @@
       <c r="F477" t="s">
         <v>7707</v>
       </c>
-    </row>
-    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G477" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H477" t="str">
+        <f t="shared" si="26"/>
+        <v>fxo_history.csv</v>
+      </c>
+    </row>
+    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>6362</v>
       </c>
@@ -67582,8 +67837,15 @@
       <c r="F478" t="s">
         <v>7708</v>
       </c>
-    </row>
-    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G478" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H478" t="str">
+        <f t="shared" si="26"/>
+        <v>fxp_history.csv</v>
+      </c>
+    </row>
+    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>6363</v>
       </c>
@@ -67599,8 +67861,15 @@
       <c r="F479" t="s">
         <v>7709</v>
       </c>
-    </row>
-    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G479" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H479" t="str">
+        <f t="shared" si="26"/>
+        <v>fxr_history.csv</v>
+      </c>
+    </row>
+    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>6364</v>
       </c>
@@ -67616,8 +67885,15 @@
       <c r="F480" t="s">
         <v>7710</v>
       </c>
-    </row>
-    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G480" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H480" t="str">
+        <f t="shared" si="26"/>
+        <v>fxs_history.csv</v>
+      </c>
+    </row>
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>6365</v>
       </c>
@@ -67633,8 +67909,15 @@
       <c r="F481" t="s">
         <v>7711</v>
       </c>
-    </row>
-    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G481" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H481" t="str">
+        <f t="shared" si="26"/>
+        <v>fxsg_history.csv</v>
+      </c>
+    </row>
+    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>6366</v>
       </c>
@@ -67650,8 +67933,15 @@
       <c r="F482" t="s">
         <v>7712</v>
       </c>
-    </row>
-    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G482" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H482" t="str">
+        <f t="shared" si="26"/>
+        <v>fxu_history.csv</v>
+      </c>
+    </row>
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>6367</v>
       </c>
@@ -67667,8 +67957,15 @@
       <c r="F483" t="s">
         <v>7713</v>
       </c>
-    </row>
-    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G483" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H483" t="str">
+        <f t="shared" si="26"/>
+        <v>fxy_history.csv</v>
+      </c>
+    </row>
+    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>6368</v>
       </c>
@@ -67684,8 +67981,15 @@
       <c r="F484" t="s">
         <v>7714</v>
       </c>
-    </row>
-    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G484" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H484" t="str">
+        <f t="shared" si="26"/>
+        <v>fxz_history.csv</v>
+      </c>
+    </row>
+    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>6369</v>
       </c>
@@ -67701,8 +68005,15 @@
       <c r="F485" t="s">
         <v>7715</v>
       </c>
-    </row>
-    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G485" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H485" t="str">
+        <f t="shared" si="26"/>
+        <v>fyc_history.csv</v>
+      </c>
+    </row>
+    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>6370</v>
       </c>
@@ -67718,8 +68029,15 @@
       <c r="F486" t="s">
         <v>7716</v>
       </c>
-    </row>
-    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G486" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H486" t="str">
+        <f t="shared" si="26"/>
+        <v>fyld_history.csv</v>
+      </c>
+    </row>
+    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>6371</v>
       </c>
@@ -67735,8 +68053,15 @@
       <c r="F487" t="s">
         <v>7717</v>
       </c>
-    </row>
-    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G487" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H487" t="str">
+        <f t="shared" si="26"/>
+        <v>fyt_history.csv</v>
+      </c>
+    </row>
+    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>6372</v>
       </c>
@@ -67752,8 +68077,15 @@
       <c r="F488" t="s">
         <v>7718</v>
       </c>
-    </row>
-    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G488" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H488" t="str">
+        <f t="shared" si="26"/>
+        <v>fyx_history.csv</v>
+      </c>
+    </row>
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>6373</v>
       </c>
@@ -67769,8 +68101,15 @@
       <c r="F489" t="s">
         <v>7719</v>
       </c>
-    </row>
-    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G489" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H489" t="str">
+        <f t="shared" si="26"/>
+        <v>gaa_history.csv</v>
+      </c>
+    </row>
+    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>6374</v>
       </c>
@@ -67783,11 +68122,21 @@
       <c r="D490" t="s">
         <v>7232</v>
       </c>
-      <c r="F490" t="s">
+      <c r="E490" t="s">
+        <v>8597</v>
+      </c>
+      <c r="F490" s="2" t="s">
         <v>7720</v>
       </c>
-    </row>
-    <row r="491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G490" s="2" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H490" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>gal_history.csv</v>
+      </c>
+    </row>
+    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>6375</v>
       </c>
@@ -67803,8 +68152,15 @@
       <c r="F491" t="s">
         <v>7721</v>
       </c>
-    </row>
-    <row r="492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G491" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H491" t="str">
+        <f t="shared" ref="H491:H554" si="27">_xlfn.CONCAT(F491,G491)</f>
+        <v>gasl_history.csv</v>
+      </c>
+    </row>
+    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>6376</v>
       </c>
@@ -67820,8 +68176,15 @@
       <c r="F492" t="s">
         <v>7722</v>
       </c>
-    </row>
-    <row r="493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G492" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H492" t="str">
+        <f t="shared" si="27"/>
+        <v>gaz_history.csv</v>
+      </c>
+    </row>
+    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>6377</v>
       </c>
@@ -67837,8 +68200,15 @@
       <c r="F493" t="s">
         <v>7723</v>
       </c>
-    </row>
-    <row r="494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G493" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H493" t="str">
+        <f t="shared" si="27"/>
+        <v>gbb_history.csv</v>
+      </c>
+    </row>
+    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>6378</v>
       </c>
@@ -67854,8 +68224,15 @@
       <c r="F494" t="s">
         <v>7724</v>
       </c>
-    </row>
-    <row r="495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G494" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H494" t="str">
+        <f t="shared" si="27"/>
+        <v>gbf_history.csv</v>
+      </c>
+    </row>
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>6379</v>
       </c>
@@ -67871,8 +68248,15 @@
       <c r="F495" t="s">
         <v>7725</v>
       </c>
-    </row>
-    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G495" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H495" t="str">
+        <f t="shared" si="27"/>
+        <v>gcc_history.csv</v>
+      </c>
+    </row>
+    <row r="496" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>6380</v>
       </c>
@@ -67888,8 +68272,15 @@
       <c r="F496" t="s">
         <v>7726</v>
       </c>
-    </row>
-    <row r="497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G496" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H496" t="str">
+        <f t="shared" si="27"/>
+        <v>gce_history.csv</v>
+      </c>
+    </row>
+    <row r="497" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>6381</v>
       </c>
@@ -67905,8 +68296,15 @@
       <c r="F497" t="s">
         <v>7727</v>
       </c>
-    </row>
-    <row r="498" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G497" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H497" t="str">
+        <f t="shared" si="27"/>
+        <v>gdx_history.csv</v>
+      </c>
+    </row>
+    <row r="498" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>6382</v>
       </c>
@@ -67922,8 +68320,15 @@
       <c r="F498" t="s">
         <v>7728</v>
       </c>
-    </row>
-    <row r="499" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G498" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H498" t="str">
+        <f t="shared" si="27"/>
+        <v>gdxj_history.csv</v>
+      </c>
+    </row>
+    <row r="499" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>6383</v>
       </c>
@@ -67939,8 +68344,15 @@
       <c r="F499" t="s">
         <v>7729</v>
       </c>
-    </row>
-    <row r="500" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G499" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H499" t="str">
+        <f t="shared" si="27"/>
+        <v>gdxs_history.csv</v>
+      </c>
+    </row>
+    <row r="500" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>6384</v>
       </c>
@@ -67956,8 +68368,15 @@
       <c r="F500" t="s">
         <v>7730</v>
       </c>
-    </row>
-    <row r="501" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G500" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H500" t="str">
+        <f t="shared" si="27"/>
+        <v>gdxx_history.csv</v>
+      </c>
+    </row>
+    <row r="501" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>6385</v>
       </c>
@@ -67973,8 +68392,15 @@
       <c r="F501" t="s">
         <v>7731</v>
       </c>
-    </row>
-    <row r="502" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G501" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H501" t="str">
+        <f t="shared" si="27"/>
+        <v>geur_history.csv</v>
+      </c>
+    </row>
+    <row r="502" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>6386</v>
       </c>
@@ -67990,8 +68416,15 @@
       <c r="F502" t="s">
         <v>7732</v>
       </c>
-    </row>
-    <row r="503" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G502" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H502" t="str">
+        <f t="shared" si="27"/>
+        <v>gex_history.csv</v>
+      </c>
+    </row>
+    <row r="503" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>6387</v>
       </c>
@@ -68007,8 +68440,15 @@
       <c r="F503" t="s">
         <v>7733</v>
       </c>
-    </row>
-    <row r="504" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G503" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H503" t="str">
+        <f t="shared" si="27"/>
+        <v>ghii_history.csv</v>
+      </c>
+    </row>
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>6388</v>
       </c>
@@ -68024,8 +68464,15 @@
       <c r="F504" t="s">
         <v>7734</v>
       </c>
-    </row>
-    <row r="505" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G504" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H504" t="str">
+        <f t="shared" si="27"/>
+        <v>gii_history.csv</v>
+      </c>
+    </row>
+    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>6389</v>
       </c>
@@ -68041,8 +68488,15 @@
       <c r="F505" t="s">
         <v>7735</v>
       </c>
-    </row>
-    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G505" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H505" t="str">
+        <f t="shared" si="27"/>
+        <v>gld_history.csv</v>
+      </c>
+    </row>
+    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>6390</v>
       </c>
@@ -68058,8 +68512,15 @@
       <c r="F506" t="s">
         <v>7736</v>
       </c>
-    </row>
-    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G506" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H506" t="str">
+        <f t="shared" si="27"/>
+        <v>gldi_history.csv</v>
+      </c>
+    </row>
+    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>6391</v>
       </c>
@@ -68075,8 +68536,15 @@
       <c r="F507" t="s">
         <v>7737</v>
       </c>
-    </row>
-    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G507" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H507" t="str">
+        <f t="shared" si="27"/>
+        <v>gll_history.csv</v>
+      </c>
+    </row>
+    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>6392</v>
       </c>
@@ -68092,8 +68560,15 @@
       <c r="F508" t="s">
         <v>7738</v>
       </c>
-    </row>
-    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G508" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H508" t="str">
+        <f t="shared" si="27"/>
+        <v>gltr_history.csv</v>
+      </c>
+    </row>
+    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>6393</v>
       </c>
@@ -68109,8 +68584,15 @@
       <c r="F509" t="s">
         <v>7739</v>
       </c>
-    </row>
-    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G509" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H509" t="str">
+        <f t="shared" si="27"/>
+        <v>gmf_history.csv</v>
+      </c>
+    </row>
+    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>6394</v>
       </c>
@@ -68126,8 +68608,15 @@
       <c r="F510" t="s">
         <v>7740</v>
       </c>
-    </row>
-    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G510" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H510" t="str">
+        <f t="shared" si="27"/>
+        <v>gmom_history.csv</v>
+      </c>
+    </row>
+    <row r="511" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>6395</v>
       </c>
@@ -68143,8 +68632,15 @@
       <c r="F511" t="s">
         <v>7741</v>
       </c>
-    </row>
-    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G511" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H511" t="str">
+        <f t="shared" si="27"/>
+        <v>gnma_history.csv</v>
+      </c>
+    </row>
+    <row r="512" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>6396</v>
       </c>
@@ -68160,8 +68656,15 @@
       <c r="F512" t="s">
         <v>7742</v>
       </c>
-    </row>
-    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G512" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H512" t="str">
+        <f t="shared" si="27"/>
+        <v>gnr_history.csv</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>6397</v>
       </c>
@@ -68177,8 +68680,15 @@
       <c r="F513" t="s">
         <v>7743</v>
       </c>
-    </row>
-    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G513" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H513" t="str">
+        <f t="shared" si="27"/>
+        <v>govt_history.csv</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>6398</v>
       </c>
@@ -68194,8 +68704,15 @@
       <c r="F514" t="s">
         <v>7744</v>
       </c>
-    </row>
-    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G514" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H514" t="str">
+        <f t="shared" si="27"/>
+        <v>gqre_history.csv</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>6399</v>
       </c>
@@ -68211,8 +68728,15 @@
       <c r="F515" t="s">
         <v>7745</v>
       </c>
-    </row>
-    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G515" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H515" t="str">
+        <f t="shared" si="27"/>
+        <v>grek_history.csv</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>6400</v>
       </c>
@@ -68228,8 +68752,15 @@
       <c r="F516" t="s">
         <v>7746</v>
       </c>
-    </row>
-    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G516" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H516" t="str">
+        <f t="shared" si="27"/>
+        <v>gres_history.csv</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>6401</v>
       </c>
@@ -68245,8 +68776,15 @@
       <c r="F517" t="s">
         <v>7747</v>
       </c>
-    </row>
-    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G517" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H517" t="str">
+        <f t="shared" si="27"/>
+        <v>gri_history.csv</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>6402</v>
       </c>
@@ -68262,8 +68800,15 @@
       <c r="F518" t="s">
         <v>7748</v>
       </c>
-    </row>
-    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G518" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H518" t="str">
+        <f t="shared" si="27"/>
+        <v>grid_history.csv</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>6403</v>
       </c>
@@ -68279,8 +68824,15 @@
       <c r="F519" t="s">
         <v>7749</v>
       </c>
-    </row>
-    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G519" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H519" t="str">
+        <f t="shared" si="27"/>
+        <v>grn_history.csv</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>6404</v>
       </c>
@@ -68296,8 +68848,15 @@
       <c r="F520" t="s">
         <v>7750</v>
       </c>
-    </row>
-    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G520" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H520" t="str">
+        <f t="shared" si="27"/>
+        <v>gru_history.csv</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>6405</v>
       </c>
@@ -68313,8 +68872,15 @@
       <c r="F521" t="s">
         <v>7751</v>
       </c>
-    </row>
-    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G521" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H521" t="str">
+        <f t="shared" si="27"/>
+        <v>grwn_history.csv</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>6406</v>
       </c>
@@ -68330,8 +68896,15 @@
       <c r="F522" t="s">
         <v>7752</v>
       </c>
-    </row>
-    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G522" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H522" t="str">
+        <f t="shared" si="27"/>
+        <v>gsc_history.csv</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>6407</v>
       </c>
@@ -68347,8 +68920,15 @@
       <c r="F523" t="s">
         <v>7753</v>
       </c>
-    </row>
-    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G523" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H523" t="str">
+        <f t="shared" si="27"/>
+        <v>gsg_history.csv</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>6408</v>
       </c>
@@ -68364,8 +68944,15 @@
       <c r="F524" t="s">
         <v>7754</v>
       </c>
-    </row>
-    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G524" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H524" t="str">
+        <f t="shared" si="27"/>
+        <v>gsp_history.csv</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>6409</v>
       </c>
@@ -68381,8 +68968,15 @@
       <c r="F525" t="s">
         <v>7755</v>
       </c>
-    </row>
-    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G525" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H525" t="str">
+        <f t="shared" si="27"/>
+        <v>gsy_history.csv</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>6410</v>
       </c>
@@ -68398,8 +68992,15 @@
       <c r="F526" t="s">
         <v>7756</v>
       </c>
-    </row>
-    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G526" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H526" t="str">
+        <f t="shared" si="27"/>
+        <v>gulf_history.csv</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>6411</v>
       </c>
@@ -68415,8 +69016,15 @@
       <c r="F527" t="s">
         <v>7757</v>
       </c>
-    </row>
-    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G527" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H527" t="str">
+        <f t="shared" si="27"/>
+        <v>gunr_history.csv</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>6412</v>
       </c>
@@ -68432,8 +69040,15 @@
       <c r="F528" t="s">
         <v>7758</v>
       </c>
-    </row>
-    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G528" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H528" t="str">
+        <f t="shared" si="27"/>
+        <v>guru_history.csv</v>
+      </c>
+    </row>
+    <row r="529" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>6413</v>
       </c>
@@ -68449,8 +69064,15 @@
       <c r="F529" t="s">
         <v>7759</v>
       </c>
-    </row>
-    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G529" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H529" t="str">
+        <f t="shared" si="27"/>
+        <v>gush_history.csv</v>
+      </c>
+    </row>
+    <row r="530" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>6414</v>
       </c>
@@ -68466,8 +69088,15 @@
       <c r="F530" t="s">
         <v>7760</v>
       </c>
-    </row>
-    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G530" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H530" t="str">
+        <f t="shared" si="27"/>
+        <v>gval_history.csv</v>
+      </c>
+    </row>
+    <row r="531" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>6415</v>
       </c>
@@ -68483,8 +69112,15 @@
       <c r="F531" t="s">
         <v>7761</v>
       </c>
-    </row>
-    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G531" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H531" t="str">
+        <f t="shared" si="27"/>
+        <v>gvi_history.csv</v>
+      </c>
+    </row>
+    <row r="532" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>6416</v>
       </c>
@@ -68500,8 +69136,15 @@
       <c r="F532" t="s">
         <v>7762</v>
       </c>
-    </row>
-    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G532" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H532" t="str">
+        <f t="shared" si="27"/>
+        <v>gwx_history.csv</v>
+      </c>
+    </row>
+    <row r="533" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>6417</v>
       </c>
@@ -68517,8 +69160,15 @@
       <c r="F533" t="s">
         <v>7763</v>
       </c>
-    </row>
-    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G533" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H533" t="str">
+        <f t="shared" si="27"/>
+        <v>gxc_history.csv</v>
+      </c>
+    </row>
+    <row r="534" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>6418</v>
       </c>
@@ -68534,8 +69184,15 @@
       <c r="F534" t="s">
         <v>7764</v>
       </c>
-    </row>
-    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G534" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H534" t="str">
+        <f t="shared" si="27"/>
+        <v>gxf_history.csv</v>
+      </c>
+    </row>
+    <row r="535" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>6419</v>
       </c>
@@ -68551,8 +69208,15 @@
       <c r="F535" t="s">
         <v>7765</v>
       </c>
-    </row>
-    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G535" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H535" t="str">
+        <f t="shared" si="27"/>
+        <v>gxg_history.csv</v>
+      </c>
+    </row>
+    <row r="536" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>6420</v>
       </c>
@@ -68568,8 +69232,15 @@
       <c r="F536" t="s">
         <v>7766</v>
       </c>
-    </row>
-    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G536" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H536" t="str">
+        <f t="shared" si="27"/>
+        <v>gyen_history.csv</v>
+      </c>
+    </row>
+    <row r="537" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>6421</v>
       </c>
@@ -68585,8 +69256,15 @@
       <c r="F537" t="s">
         <v>7767</v>
       </c>
-    </row>
-    <row r="538" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G537" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H537" t="str">
+        <f t="shared" si="27"/>
+        <v>gyld_history.csv</v>
+      </c>
+    </row>
+    <row r="538" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>6422</v>
       </c>
@@ -68602,8 +69280,15 @@
       <c r="F538" t="s">
         <v>7768</v>
       </c>
-    </row>
-    <row r="539" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G538" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H538" t="str">
+        <f t="shared" si="27"/>
+        <v>hao_history.csv</v>
+      </c>
+    </row>
+    <row r="539" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>6423</v>
       </c>
@@ -68619,8 +69304,15 @@
       <c r="F539" t="s">
         <v>7769</v>
       </c>
-    </row>
-    <row r="540" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G539" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H539" t="str">
+        <f t="shared" si="27"/>
+        <v>hap_history.csv</v>
+      </c>
+    </row>
+    <row r="540" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>6424</v>
       </c>
@@ -68633,11 +69325,18 @@
       <c r="D540" t="s">
         <v>7232</v>
       </c>
-      <c r="F540" t="s">
+      <c r="F540" s="2" t="s">
         <v>7770</v>
       </c>
-    </row>
-    <row r="541" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G540" s="2" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H540" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>hdg_history.csv</v>
+      </c>
+    </row>
+    <row r="541" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>6425</v>
       </c>
@@ -68653,8 +69352,15 @@
       <c r="F541" t="s">
         <v>7771</v>
       </c>
-    </row>
-    <row r="542" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G541" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H541" t="str">
+        <f t="shared" ref="H541" si="28">_xlfn.CONCAT(F541,G541)</f>
+        <v>hdge_history.csv</v>
+      </c>
+    </row>
+    <row r="542" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>6426</v>
       </c>
@@ -68671,7 +69377,7 @@
         <v>7772</v>
       </c>
     </row>
-    <row r="543" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>6427</v>
       </c>
@@ -68688,7 +69394,7 @@
         <v>7773</v>
       </c>
     </row>
-    <row r="544" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>6428</v>
       </c>

</xml_diff>

<commit_message>
add sentiment analysis file
</commit_message>
<xml_diff>
--- a/tickers.xlsx
+++ b/tickers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttbon\Desktop\stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C85242E-DC9B-44C7-B668-6A544B4B7C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534742B7-186F-4324-A973-733682138E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4470" yWindow="1620" windowWidth="16080" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7260" yWindow="1905" windowWidth="16080" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tickers" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13205" uniqueCount="8598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13255" uniqueCount="8598">
   <si>
     <t>tickers</t>
   </si>
@@ -56404,8 +56404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA55E37D-5D70-4D70-8000-B4CA16A6A6A0}">
   <dimension ref="A1:H1345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
-      <selection activeCell="E491" sqref="E491"/>
+    <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
+      <selection activeCell="E590" sqref="E590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67289,7 +67289,7 @@
         <v>5885</v>
       </c>
       <c r="H455" t="str">
-        <f t="shared" ref="H454:H455" si="23">_xlfn.CONCAT(F455,G455)</f>
+        <f t="shared" ref="H455" si="23">_xlfn.CONCAT(F455,G455)</f>
         <v>fud_history.csv</v>
       </c>
     </row>
@@ -68156,7 +68156,7 @@
         <v>5885</v>
       </c>
       <c r="H491" t="str">
-        <f t="shared" ref="H491:H554" si="27">_xlfn.CONCAT(F491,G491)</f>
+        <f t="shared" ref="H491:H540" si="27">_xlfn.CONCAT(F491,G491)</f>
         <v>gasl_history.csv</v>
       </c>
     </row>
@@ -69376,6 +69376,13 @@
       <c r="F542" t="s">
         <v>7772</v>
       </c>
+      <c r="G542" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H542" t="str">
+        <f t="shared" ref="H542:H585" si="29">_xlfn.CONCAT(F542,G542)</f>
+        <v>hdv_history.csv</v>
+      </c>
     </row>
     <row r="543" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
@@ -69393,6 +69400,13 @@
       <c r="F543" t="s">
         <v>7773</v>
       </c>
+      <c r="G543" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H543" t="str">
+        <f t="shared" si="29"/>
+        <v>heco_history.csv</v>
+      </c>
     </row>
     <row r="544" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
@@ -69410,8 +69424,15 @@
       <c r="F544" t="s">
         <v>7774</v>
       </c>
-    </row>
-    <row r="545" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G544" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H544" t="str">
+        <f t="shared" si="29"/>
+        <v>hedj_history.csv</v>
+      </c>
+    </row>
+    <row r="545" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>6429</v>
       </c>
@@ -69427,8 +69448,15 @@
       <c r="F545" t="s">
         <v>7775</v>
       </c>
-    </row>
-    <row r="546" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G545" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H545" t="str">
+        <f t="shared" si="29"/>
+        <v>heem_history.csv</v>
+      </c>
+    </row>
+    <row r="546" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>6430</v>
       </c>
@@ -69444,8 +69472,15 @@
       <c r="F546" t="s">
         <v>7776</v>
       </c>
-    </row>
-    <row r="547" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G546" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H546" t="str">
+        <f t="shared" si="29"/>
+        <v>hefa_history.csv</v>
+      </c>
+    </row>
+    <row r="547" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>6431</v>
       </c>
@@ -69461,8 +69496,15 @@
       <c r="F547" t="s">
         <v>7777</v>
       </c>
-    </row>
-    <row r="548" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G547" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H547" t="str">
+        <f t="shared" si="29"/>
+        <v>hevy_history.csv</v>
+      </c>
+    </row>
+    <row r="548" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>6432</v>
       </c>
@@ -69478,8 +69520,15 @@
       <c r="F548" t="s">
         <v>7778</v>
       </c>
-    </row>
-    <row r="549" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G548" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H548" t="str">
+        <f t="shared" si="29"/>
+        <v>hewg_history.csv</v>
+      </c>
+    </row>
+    <row r="549" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>6433</v>
       </c>
@@ -69495,8 +69544,15 @@
       <c r="F549" t="s">
         <v>7779</v>
       </c>
-    </row>
-    <row r="550" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G549" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H549" t="str">
+        <f t="shared" si="29"/>
+        <v>hewj_history.csv</v>
+      </c>
+    </row>
+    <row r="550" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>6434</v>
       </c>
@@ -69512,8 +69568,15 @@
       <c r="F550" t="s">
         <v>7780</v>
       </c>
-    </row>
-    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G550" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H550" t="str">
+        <f t="shared" si="29"/>
+        <v>hezu_history.csv</v>
+      </c>
+    </row>
+    <row r="551" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>6435</v>
       </c>
@@ -69529,8 +69592,15 @@
       <c r="F551" t="s">
         <v>7781</v>
       </c>
-    </row>
-    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G551" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H551" t="str">
+        <f t="shared" si="29"/>
+        <v>hgi_history.csv</v>
+      </c>
+    </row>
+    <row r="552" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>6436</v>
       </c>
@@ -69546,8 +69616,15 @@
       <c r="F552" t="s">
         <v>7782</v>
       </c>
-    </row>
-    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G552" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H552" t="str">
+        <f t="shared" si="29"/>
+        <v>hilo_history.csv</v>
+      </c>
+    </row>
+    <row r="553" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>6437</v>
       </c>
@@ -69563,8 +69640,15 @@
       <c r="F553" t="s">
         <v>7783</v>
       </c>
-    </row>
-    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G553" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H553" t="str">
+        <f t="shared" si="29"/>
+        <v>hold_history.csv</v>
+      </c>
+    </row>
+    <row r="554" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>6438</v>
       </c>
@@ -69580,8 +69664,15 @@
       <c r="F554" t="s">
         <v>7784</v>
       </c>
-    </row>
-    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G554" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H554" t="str">
+        <f t="shared" si="29"/>
+        <v>hspx_history.csv</v>
+      </c>
+    </row>
+    <row r="555" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>6439</v>
       </c>
@@ -69597,8 +69688,15 @@
       <c r="F555" t="s">
         <v>7785</v>
       </c>
-    </row>
-    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G555" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H555" t="str">
+        <f t="shared" si="29"/>
+        <v>huse_history.csv</v>
+      </c>
+    </row>
+    <row r="556" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>6440</v>
       </c>
@@ -69614,8 +69712,15 @@
       <c r="F556" t="s">
         <v>7786</v>
       </c>
-    </row>
-    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G556" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H556" t="str">
+        <f t="shared" si="29"/>
+        <v>hyd_history.csv</v>
+      </c>
+    </row>
+    <row r="557" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>6441</v>
       </c>
@@ -69631,8 +69736,15 @@
       <c r="F557" t="s">
         <v>7787</v>
       </c>
-    </row>
-    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G557" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H557" t="str">
+        <f t="shared" si="29"/>
+        <v>hyem_history.csv</v>
+      </c>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>6442</v>
       </c>
@@ -69648,8 +69760,15 @@
       <c r="F558" t="s">
         <v>7788</v>
       </c>
-    </row>
-    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G558" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H558" t="str">
+        <f t="shared" si="29"/>
+        <v>hyg_history.csv</v>
+      </c>
+    </row>
+    <row r="559" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>6443</v>
       </c>
@@ -69665,8 +69784,15 @@
       <c r="F559" t="s">
         <v>7789</v>
       </c>
-    </row>
-    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G559" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H559" t="str">
+        <f t="shared" si="29"/>
+        <v>hygh_history.csv</v>
+      </c>
+    </row>
+    <row r="560" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>6444</v>
       </c>
@@ -69682,8 +69808,15 @@
       <c r="F560" t="s">
         <v>7790</v>
       </c>
-    </row>
-    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G560" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H560" t="str">
+        <f t="shared" si="29"/>
+        <v>hyih_history.csv</v>
+      </c>
+    </row>
+    <row r="561" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
         <v>6445</v>
       </c>
@@ -69699,8 +69832,15 @@
       <c r="F561" t="s">
         <v>7791</v>
       </c>
-    </row>
-    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G561" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H561" t="str">
+        <f t="shared" si="29"/>
+        <v>hyld_history.csv</v>
+      </c>
+    </row>
+    <row r="562" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
         <v>6446</v>
       </c>
@@ -69716,8 +69856,15 @@
       <c r="F562" t="s">
         <v>7792</v>
       </c>
-    </row>
-    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G562" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H562" t="str">
+        <f t="shared" si="29"/>
+        <v>hyls_history.csv</v>
+      </c>
+    </row>
+    <row r="563" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
         <v>6447</v>
       </c>
@@ -69733,8 +69880,15 @@
       <c r="F563" t="s">
         <v>7793</v>
       </c>
-    </row>
-    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G563" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H563" t="str">
+        <f t="shared" si="29"/>
+        <v>hymb_history.csv</v>
+      </c>
+    </row>
+    <row r="564" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
         <v>6448</v>
       </c>
@@ -69750,8 +69904,15 @@
       <c r="F564" t="s">
         <v>7794</v>
       </c>
-    </row>
-    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G564" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H564" t="str">
+        <f t="shared" si="29"/>
+        <v>hynd_history.csv</v>
+      </c>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
         <v>6449</v>
       </c>
@@ -69767,8 +69928,15 @@
       <c r="F565" t="s">
         <v>7795</v>
       </c>
-    </row>
-    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G565" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H565" t="str">
+        <f t="shared" si="29"/>
+        <v>hys_history.csv</v>
+      </c>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
         <v>6450</v>
       </c>
@@ -69784,8 +69952,15 @@
       <c r="F566" t="s">
         <v>7796</v>
       </c>
-    </row>
-    <row r="567" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G566" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H566" t="str">
+        <f t="shared" si="29"/>
+        <v>hyzd_history.csv</v>
+      </c>
+    </row>
+    <row r="567" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
         <v>6451</v>
       </c>
@@ -69801,8 +69976,15 @@
       <c r="F567" t="s">
         <v>7797</v>
       </c>
-    </row>
-    <row r="568" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G567" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H567" t="str">
+        <f t="shared" si="29"/>
+        <v>iai_history.csv</v>
+      </c>
+    </row>
+    <row r="568" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
         <v>6452</v>
       </c>
@@ -69818,8 +70000,15 @@
       <c r="F568" t="s">
         <v>7798</v>
       </c>
-    </row>
-    <row r="569" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G568" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H568" t="str">
+        <f t="shared" si="29"/>
+        <v>iak_history.csv</v>
+      </c>
+    </row>
+    <row r="569" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
         <v>6453</v>
       </c>
@@ -69835,8 +70024,15 @@
       <c r="F569" t="s">
         <v>7799</v>
       </c>
-    </row>
-    <row r="570" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G569" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H569" t="str">
+        <f t="shared" si="29"/>
+        <v>iat_history.csv</v>
+      </c>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
         <v>6454</v>
       </c>
@@ -69852,8 +70048,15 @@
       <c r="F570" t="s">
         <v>7800</v>
       </c>
-    </row>
-    <row r="571" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G570" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H570" t="str">
+        <f t="shared" si="29"/>
+        <v>iau_history.csv</v>
+      </c>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
         <v>6455</v>
       </c>
@@ -69869,8 +70072,15 @@
       <c r="F571" t="s">
         <v>7801</v>
       </c>
-    </row>
-    <row r="572" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G571" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H571" t="str">
+        <f t="shared" si="29"/>
+        <v>ibb_history.csv</v>
+      </c>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
         <v>6456</v>
       </c>
@@ -69886,8 +70096,15 @@
       <c r="F572" t="s">
         <v>7802</v>
       </c>
-    </row>
-    <row r="573" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G572" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H572" t="str">
+        <f t="shared" si="29"/>
+        <v>ibcc_history.csv</v>
+      </c>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
         <v>6457</v>
       </c>
@@ -69903,8 +70120,15 @@
       <c r="F573" t="s">
         <v>7803</v>
       </c>
-    </row>
-    <row r="574" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G573" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H573" t="str">
+        <f t="shared" si="29"/>
+        <v>ibcd_history.csv</v>
+      </c>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
         <v>6458</v>
       </c>
@@ -69920,8 +70144,15 @@
       <c r="F574" t="s">
         <v>7804</v>
       </c>
-    </row>
-    <row r="575" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G574" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H574" t="str">
+        <f t="shared" si="29"/>
+        <v>ibce_history.csv</v>
+      </c>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
         <v>6459</v>
       </c>
@@ -69937,8 +70168,15 @@
       <c r="F575" t="s">
         <v>7805</v>
       </c>
-    </row>
-    <row r="576" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G575" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H575" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdb_history.csv</v>
+      </c>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
         <v>6460</v>
       </c>
@@ -69954,8 +70192,15 @@
       <c r="F576" t="s">
         <v>7806</v>
       </c>
-    </row>
-    <row r="577" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G576" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H576" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdc_history.csv</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
         <v>6461</v>
       </c>
@@ -69971,8 +70216,15 @@
       <c r="F577" t="s">
         <v>7807</v>
       </c>
-    </row>
-    <row r="578" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G577" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H577" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdd_history.csv</v>
+      </c>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
         <v>6462</v>
       </c>
@@ -69988,8 +70240,15 @@
       <c r="F578" t="s">
         <v>7808</v>
       </c>
-    </row>
-    <row r="579" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G578" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H578" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdh_history.csv</v>
+      </c>
+    </row>
+    <row r="579" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
         <v>6463</v>
       </c>
@@ -70005,8 +70264,15 @@
       <c r="F579" t="s">
         <v>7809</v>
       </c>
-    </row>
-    <row r="580" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G579" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H579" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdj_history.csv</v>
+      </c>
+    </row>
+    <row r="580" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
         <v>6464</v>
       </c>
@@ -70022,8 +70288,15 @@
       <c r="F580" t="s">
         <v>7810</v>
       </c>
-    </row>
-    <row r="581" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G580" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H580" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdk_history.csv</v>
+      </c>
+    </row>
+    <row r="581" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
         <v>6465</v>
       </c>
@@ -70039,8 +70312,15 @@
       <c r="F581" t="s">
         <v>7811</v>
       </c>
-    </row>
-    <row r="582" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G581" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H581" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdl_history.csv</v>
+      </c>
+    </row>
+    <row r="582" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
         <v>6466</v>
       </c>
@@ -70056,8 +70336,15 @@
       <c r="F582" t="s">
         <v>7812</v>
       </c>
-    </row>
-    <row r="583" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G582" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H582" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdm_history.csv</v>
+      </c>
+    </row>
+    <row r="583" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
         <v>6467</v>
       </c>
@@ -70073,8 +70360,15 @@
       <c r="F583" t="s">
         <v>7813</v>
       </c>
-    </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G583" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H583" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdn_history.csv</v>
+      </c>
+    </row>
+    <row r="584" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
         <v>6468</v>
       </c>
@@ -70090,8 +70384,15 @@
       <c r="F584" t="s">
         <v>7814</v>
       </c>
-    </row>
-    <row r="585" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G584" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H584" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdo_history.csv</v>
+      </c>
+    </row>
+    <row r="585" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
         <v>6469</v>
       </c>
@@ -70107,8 +70408,15 @@
       <c r="F585" t="s">
         <v>7815</v>
       </c>
-    </row>
-    <row r="586" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G585" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H585" t="str">
+        <f t="shared" si="29"/>
+        <v>ibdp_history.csv</v>
+      </c>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>6470</v>
       </c>
@@ -70124,8 +70432,15 @@
       <c r="F586" t="s">
         <v>7816</v>
       </c>
-    </row>
-    <row r="587" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G586" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H586" t="str">
+        <f t="shared" ref="H586:H591" si="30">_xlfn.CONCAT(F586,G586)</f>
+        <v>ibdq_history.csv</v>
+      </c>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A587" t="s">
         <v>6471</v>
       </c>
@@ -70141,8 +70456,15 @@
       <c r="F587" t="s">
         <v>7817</v>
       </c>
-    </row>
-    <row r="588" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G587" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H587" t="str">
+        <f t="shared" si="30"/>
+        <v>ibln_history.csv</v>
+      </c>
+    </row>
+    <row r="588" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A588" t="s">
         <v>6472</v>
       </c>
@@ -70158,8 +70480,15 @@
       <c r="F588" t="s">
         <v>7818</v>
       </c>
-    </row>
-    <row r="589" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G588" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H588" t="str">
+        <f t="shared" si="30"/>
+        <v>ibmg_history.csv</v>
+      </c>
+    </row>
+    <row r="589" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A589" t="s">
         <v>6473</v>
       </c>
@@ -70175,8 +70504,15 @@
       <c r="F589" t="s">
         <v>7819</v>
       </c>
-    </row>
-    <row r="590" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G589" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H589" t="str">
+        <f t="shared" si="30"/>
+        <v>ibmh_history.csv</v>
+      </c>
+    </row>
+    <row r="590" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
         <v>6474</v>
       </c>
@@ -70189,11 +70525,18 @@
       <c r="D590" t="s">
         <v>7232</v>
       </c>
-      <c r="F590" t="s">
+      <c r="F590" s="2" t="s">
         <v>7820</v>
       </c>
-    </row>
-    <row r="591" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G590" s="2" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H590" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>ibmi_history.csv</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
         <v>6475</v>
       </c>
@@ -70209,8 +70552,15 @@
       <c r="F591" t="s">
         <v>7821</v>
       </c>
-    </row>
-    <row r="592" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G591" t="s">
+        <v>5885</v>
+      </c>
+      <c r="H591" t="str">
+        <f t="shared" si="30"/>
+        <v>ibnd_history.csv</v>
+      </c>
+    </row>
+    <row r="592" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
         <v>6476</v>
       </c>

</xml_diff>